<commit_message>
update benchmark test result
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="ardb" localSheetId="0">Sheet2!$A$2:$B$16</definedName>
-    <definedName name="redis" localSheetId="0">Sheet2!$C$2:$C$16</definedName>
+    <definedName name="redis" localSheetId="0">Sheet2!$D$2:$D$16</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>PING_INLINE</t>
   </si>
@@ -89,21 +92,30 @@
     <t>MSET (10 keys)</t>
   </si>
   <si>
+    <t>Redis</t>
+  </si>
+  <si>
     <t>Ardb-LevelDB</t>
-  </si>
-  <si>
-    <t>Redis</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ardb-LMDB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPUSH(for LRANGE)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -112,7 +124,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -121,7 +133,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -155,11 +174,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -168,55 +187,13 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="zh-CN"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Requests per second</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" baseline="0"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
+    <c:plotArea>
       <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0734561048721369"/>
-          <c:y val="0.0367196157771945"/>
-          <c:w val="0.861394353754561"/>
-          <c:h val="0.907084032528721"/>
-        </c:manualLayout>
-      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -231,7 +208,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$2:$A$16</c:f>
@@ -265,7 +241,7 @@
                   <c:v>SPOP</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>LPUSH</c:v>
+                  <c:v>LPUSH(for LRANGE)</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>LRANGE_100 (first 100 elements)</c:v>
@@ -292,49 +268,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>158730.16</c:v>
+                  <c:v>90682.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>161290.33</c:v>
+                  <c:v>92039.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90859.53</c:v>
+                  <c:v>49030.18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128279.13</c:v>
+                  <c:v>50949.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79841.59</c:v>
+                  <c:v>32067.83</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70312.61</c:v>
+                  <c:v>26702.13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41666.67</c:v>
+                  <c:v>7395.19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34708.96</c:v>
+                  <c:v>11958.49</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34588.91</c:v>
+                  <c:v>109.32599999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72674.41</c:v>
+                  <c:v>19161.13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15262.52</c:v>
+                  <c:v>6796.99</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5015.8</c:v>
+                  <c:v>2374.41</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3430.06</c:v>
+                  <c:v>1650.37</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2614.72</c:v>
+                  <c:v>1345.24</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12923.24</c:v>
+                  <c:v>5472.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,12 +325,11 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Redis</c:v>
+                  <c:v>Ardb-LMDB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet2!$A$2:$A$16</c:f>
@@ -388,7 +363,7 @@
                   <c:v>SPOP</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>LPUSH</c:v>
+                  <c:v>LPUSH(for LRANGE)</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>LRANGE_100 (first 100 elements)</c:v>
@@ -415,205 +390,218 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>156250.0</c:v>
+                  <c:v>90020.34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>163934.42</c:v>
+                  <c:v>92506.94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140845.06</c:v>
+                  <c:v>62066.71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149253.73</c:v>
+                  <c:v>87973.19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149253.73</c:v>
+                  <c:v>48217.17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>161290.33</c:v>
+                  <c:v>15689.55</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>161290.33</c:v>
+                  <c:v>9658.43</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>149253.73</c:v>
+                  <c:v>16065.06</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>153846.16</c:v>
+                  <c:v>17067.09</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>161290.33</c:v>
+                  <c:v>15705.01</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49019.61</c:v>
+                  <c:v>13343.12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21008.4</c:v>
+                  <c:v>4751.47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14684.29</c:v>
+                  <c:v>3004.68</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11312.22</c:v>
+                  <c:v>2505.98</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>54347.82</c:v>
+                  <c:v>4794.2299999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2098555016"/>
-        <c:axId val="2098364504"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$2:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>PING_INLINE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PING_BULK</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SET</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GET</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>INCR</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LPUSH</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LPOP</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SADD</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SPOP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>LPUSH(for LRANGE)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>LRANGE_100 (first 100 elements)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>LRANGE_300 (first 300 elements)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>LRANGE_500 (first 450 elements)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>LRANGE_600 (first 600 elements)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>MSET (10 keys)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>76523.39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87438.58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71850.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79349.960000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79298.37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77643.97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77026.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76780.740000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70997.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79808.460000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38269.61</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15735.71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12432.77</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9586.19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35967.599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="102506880"/>
+        <c:axId val="102753024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2098555016"/>
+        <c:axId val="102506880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098364504"/>
+        <c:crossAx val="102753024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2098364504"/>
+        <c:axId val="102753024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Throughput(q/s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US">
-                  <a:effectLst/>
-                </a:endParaRPr>
-              </a:p>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098555016"/>
+        <c:crossAx val="102506880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.875667928803981"/>
-          <c:y val="0.552866360454943"/>
-          <c:w val="0.114640792851713"/>
-          <c:h val="0.0882259689391436"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -621,20 +609,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>638174</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>790574</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="8" name="图表 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -650,6 +638,236 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.43541</cdr:x>
+      <cdr:y>0.03529</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.65837</cdr:x>
+      <cdr:y>0.10756</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4333876" y="200026"/>
+          <a:ext cx="2219325" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Request per second</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Ardb-LevelDB</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Redis</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>PING_INLINE</v>
+          </cell>
+          <cell r="B2">
+            <v>158730.16</v>
+          </cell>
+          <cell r="C2">
+            <v>156250</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>PING_BULK</v>
+          </cell>
+          <cell r="B3">
+            <v>161290.32999999999</v>
+          </cell>
+          <cell r="C3">
+            <v>163934.42000000001</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>SET</v>
+          </cell>
+          <cell r="B4">
+            <v>90859.53</v>
+          </cell>
+          <cell r="C4">
+            <v>140845.06</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>GET</v>
+          </cell>
+          <cell r="B5">
+            <v>128279.13</v>
+          </cell>
+          <cell r="C5">
+            <v>149253.73000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>INCR</v>
+          </cell>
+          <cell r="B6">
+            <v>79841.59</v>
+          </cell>
+          <cell r="C6">
+            <v>149253.73000000001</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>LPUSH</v>
+          </cell>
+          <cell r="B7">
+            <v>70312.61</v>
+          </cell>
+          <cell r="C7">
+            <v>161290.32999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>LPOP</v>
+          </cell>
+          <cell r="B8">
+            <v>41666.67</v>
+          </cell>
+          <cell r="C8">
+            <v>161290.32999999999</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>SADD</v>
+          </cell>
+          <cell r="B9">
+            <v>34708.959999999999</v>
+          </cell>
+          <cell r="C9">
+            <v>149253.73000000001</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>SPOP</v>
+          </cell>
+          <cell r="B10">
+            <v>34588.910000000003</v>
+          </cell>
+          <cell r="C10">
+            <v>153846.16</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>LPUSH</v>
+          </cell>
+          <cell r="B11">
+            <v>72674.41</v>
+          </cell>
+          <cell r="C11">
+            <v>161290.32999999999</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>LRANGE_100 (first 100 elements)</v>
+          </cell>
+          <cell r="B12">
+            <v>15262.52</v>
+          </cell>
+          <cell r="C12">
+            <v>49019.61</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>LRANGE_300 (first 300 elements)</v>
+          </cell>
+          <cell r="B13">
+            <v>5015.8</v>
+          </cell>
+          <cell r="C13">
+            <v>21008.400000000001</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>LRANGE_500 (first 450 elements)</v>
+          </cell>
+          <cell r="B14">
+            <v>3430.06</v>
+          </cell>
+          <cell r="C14">
+            <v>14684.29</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>LRANGE_600 (first 600 elements)</v>
+          </cell>
+          <cell r="B15">
+            <v>2614.7199999999998</v>
+          </cell>
+          <cell r="C15">
+            <v>11312.22</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>MSET (10 keys)</v>
+          </cell>
+          <cell r="B16">
+            <v>12923.24</v>
+          </cell>
+          <cell r="C16">
+            <v>54347.82</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -981,194 +1199,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.375" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>158730.16</v>
+        <v>90682.38</v>
       </c>
       <c r="C2">
-        <v>156250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>90020.34</v>
+      </c>
+      <c r="D2">
+        <v>76523.39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>161290.32999999999</v>
+        <v>92039.51</v>
       </c>
       <c r="C3">
-        <v>163934.42000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>92506.94</v>
+      </c>
+      <c r="D3">
+        <v>87438.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>90859.53</v>
+        <v>49030.18</v>
       </c>
       <c r="C4">
-        <v>140845.06</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>62066.71</v>
+      </c>
+      <c r="D4">
+        <v>71850.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>128279.13</v>
+        <v>50949.18</v>
       </c>
       <c r="C5">
-        <v>149253.73000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>87973.19</v>
+      </c>
+      <c r="D5">
+        <v>79349.960000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>79841.59</v>
+        <v>32067.83</v>
       </c>
       <c r="C6">
-        <v>149253.73000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>48217.17</v>
+      </c>
+      <c r="D6">
+        <v>79298.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>70312.61</v>
+        <v>26702.13</v>
       </c>
       <c r="C7">
-        <v>161290.32999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>15689.55</v>
+      </c>
+      <c r="D7">
+        <v>77643.97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>41666.67</v>
+        <v>7395.19</v>
       </c>
       <c r="C8">
-        <v>161290.32999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>9658.43</v>
+      </c>
+      <c r="D8">
+        <v>77026.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>34708.959999999999</v>
+        <v>11958.49</v>
       </c>
       <c r="C9">
-        <v>149253.73000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>16065.06</v>
+      </c>
+      <c r="D9">
+        <v>76780.740000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>34588.910000000003</v>
+        <v>109.32599999999999</v>
       </c>
       <c r="C10">
-        <v>153846.16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>17067.09</v>
+      </c>
+      <c r="D10">
+        <v>70997.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>72674.41</v>
+        <v>19161.13</v>
       </c>
       <c r="C11">
-        <v>161290.32999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>15705.01</v>
+      </c>
+      <c r="D11">
+        <v>79808.460000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12">
-        <v>15262.52</v>
+        <v>6796.99</v>
       </c>
       <c r="C12">
-        <v>49019.61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>13343.12</v>
+      </c>
+      <c r="D12">
+        <v>38269.61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
-        <v>5015.8</v>
+        <v>2374.41</v>
       </c>
       <c r="C13">
-        <v>21008.400000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>4751.47</v>
+      </c>
+      <c r="D13">
+        <v>15735.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14">
-        <v>3430.06</v>
+        <v>1650.37</v>
       </c>
       <c r="C14">
-        <v>14684.29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>3004.68</v>
+      </c>
+      <c r="D14">
+        <v>12432.77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15">
-        <v>2614.7199999999998</v>
+        <v>1345.24</v>
       </c>
       <c r="C15">
-        <v>11312.22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>2505.98</v>
+      </c>
+      <c r="D15">
+        <v>9586.19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16">
-        <v>12923.24</v>
+        <v>5472.67</v>
       </c>
       <c r="C16">
-        <v>54347.82</v>
+        <v>4794.2299999999996</v>
+      </c>
+      <c r="D16">
+        <v>35967.599999999999</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
@@ -1180,13 +1448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
add benchamrk data for rocksdb
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -10,12 +10,10 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="ardb" localSheetId="0">Sheet2!$A$2:$B$16</definedName>
     <definedName name="redis" localSheetId="0">Sheet2!$D$2:$D$16</definedName>
+    <definedName name="redis_1" localSheetId="0">Sheet2!$E$2:$E$16</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -44,11 +42,19 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="redis.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:wqy:Desktop:Code:redis.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>PING_INLINE</t>
   </si>
@@ -93,17 +99,21 @@
   </si>
   <si>
     <t>Redis</t>
+  </si>
+  <si>
+    <t>Ardb-LMDB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPUSH(for LRANGE)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Ardb-LevelDB</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Ardb-LMDB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LPUSH(for LRANGE)</t>
+    <t>Ardb-RocksDB</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -268,49 +278,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>90682.38</c:v>
+                  <c:v>95075.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92039.51</c:v>
+                  <c:v>99265.43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49030.18</c:v>
+                  <c:v>62361.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50949.18</c:v>
+                  <c:v>69045.990000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32067.83</c:v>
+                  <c:v>47572.160000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26702.13</c:v>
+                  <c:v>47369.57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7395.19</c:v>
+                  <c:v>14205.29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11958.49</c:v>
+                  <c:v>37583.39</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>109.32599999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19161.13</c:v>
+                  <c:v>49504.95</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6796.99</c:v>
+                  <c:v>7981.99</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2374.41</c:v>
+                  <c:v>3829.91</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1650.37</c:v>
+                  <c:v>2504.61</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1345.24</c:v>
+                  <c:v>1734.72</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5472.67</c:v>
+                  <c:v>9675.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -390,49 +400,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>90020.34</c:v>
+                  <c:v>91945.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92506.94</c:v>
+                  <c:v>92988.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62066.71</c:v>
+                  <c:v>72490.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87973.19</c:v>
+                  <c:v>93805.119999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48217.17</c:v>
+                  <c:v>59805.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15689.55</c:v>
+                  <c:v>27713.11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9658.43</c:v>
+                  <c:v>14711.51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16065.06</c:v>
+                  <c:v>41779.82</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17067.09</c:v>
+                  <c:v>17614.32</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15705.01</c:v>
+                  <c:v>16998.71</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13343.12</c:v>
+                  <c:v>17639.79</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4751.47</c:v>
+                  <c:v>6578.86</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3004.68</c:v>
+                  <c:v>4552.0600000000004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2505.98</c:v>
+                  <c:v>3082.94</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4794.2299999999996</c:v>
+                  <c:v>7204.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -447,7 +457,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Redis</c:v>
+                  <c:v>Ardb-RocksDB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -512,72 +522,194 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>76523.39</c:v>
+                  <c:v>92274.76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87438.58</c:v>
+                  <c:v>95721.27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71850.44</c:v>
+                  <c:v>55567.91</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79349.960000000006</c:v>
+                  <c:v>68078.16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79298.37</c:v>
+                  <c:v>34883.32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>77643.97</c:v>
+                  <c:v>40584.42</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>77026.77</c:v>
+                  <c:v>10088.27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>76780.740000000005</c:v>
+                  <c:v>24421.81</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70997.52</c:v>
+                  <c:v>87.634</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>79808.460000000006</c:v>
+                  <c:v>40719.93</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38269.61</c:v>
+                  <c:v>7445.68</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15735.71</c:v>
+                  <c:v>3113.99</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12432.77</c:v>
+                  <c:v>2156.08</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9586.19</c:v>
+                  <c:v>1650.46</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35967.599999999999</c:v>
+                  <c:v>5255.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="102506880"/>
-        <c:axId val="102753024"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Redis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$2:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>PING_INLINE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PING_BULK</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SET</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GET</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>INCR</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LPUSH</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LPOP</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SADD</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SPOP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>LPUSH(for LRANGE)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>LRANGE_100 (first 100 elements)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>LRANGE_300 (first 300 elements)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>LRANGE_500 (first 450 elements)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>LRANGE_600 (first 600 elements)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>MSET (10 keys)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>79669.850000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90044.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73692.509999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82459.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74940.61</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105466.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105797.72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100405.64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>75253.039999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87989.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45831.61</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17608.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12345.07</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7906.01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35967.599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="77774848"/>
+        <c:axId val="77776384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102506880"/>
+        <c:axId val="77774848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102753024"/>
+        <c:crossAx val="77776384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102753024"/>
+        <c:axId val="77776384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,7 +717,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102506880"/>
+        <c:crossAx val="77774848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -598,7 +730,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -610,19 +742,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>638174</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>19048</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>790574</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="图表 7"/>
+        <xdr:cNvPr id="3" name="图表 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -644,12 +776,44 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.43541</cdr:x>
-      <cdr:y>0.03529</cdr:y>
+      <cdr:x>0.3902</cdr:x>
+      <cdr:y>0.05428</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.65837</cdr:x>
-      <cdr:y>0.10756</cdr:y>
+      <cdr:x>0.50612</cdr:x>
+      <cdr:y>0.09046</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4552950" y="314327"/>
+          <a:ext cx="1352550" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.39347</cdr:x>
+      <cdr:y>0.04605</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.6</cdr:x>
+      <cdr:y>0.10362</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -658,8 +822,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4333876" y="200026"/>
-          <a:ext cx="2219325" cy="409575"/>
+          <a:off x="4591050" y="266702"/>
+          <a:ext cx="2409825" cy="333375"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -671,7 +835,11 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-            <a:t>Request per second</a:t>
+            <a:t>Request</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0"/>
+            <a:t> per second</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
@@ -681,201 +849,16 @@
 </c:userShapes>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Ardb-LevelDB</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Redis</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>PING_INLINE</v>
-          </cell>
-          <cell r="B2">
-            <v>158730.16</v>
-          </cell>
-          <cell r="C2">
-            <v>156250</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>PING_BULK</v>
-          </cell>
-          <cell r="B3">
-            <v>161290.32999999999</v>
-          </cell>
-          <cell r="C3">
-            <v>163934.42000000001</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>SET</v>
-          </cell>
-          <cell r="B4">
-            <v>90859.53</v>
-          </cell>
-          <cell r="C4">
-            <v>140845.06</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>GET</v>
-          </cell>
-          <cell r="B5">
-            <v>128279.13</v>
-          </cell>
-          <cell r="C5">
-            <v>149253.73000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>INCR</v>
-          </cell>
-          <cell r="B6">
-            <v>79841.59</v>
-          </cell>
-          <cell r="C6">
-            <v>149253.73000000001</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>LPUSH</v>
-          </cell>
-          <cell r="B7">
-            <v>70312.61</v>
-          </cell>
-          <cell r="C7">
-            <v>161290.32999999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>LPOP</v>
-          </cell>
-          <cell r="B8">
-            <v>41666.67</v>
-          </cell>
-          <cell r="C8">
-            <v>161290.32999999999</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>SADD</v>
-          </cell>
-          <cell r="B9">
-            <v>34708.959999999999</v>
-          </cell>
-          <cell r="C9">
-            <v>149253.73000000001</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>SPOP</v>
-          </cell>
-          <cell r="B10">
-            <v>34588.910000000003</v>
-          </cell>
-          <cell r="C10">
-            <v>153846.16</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>LPUSH</v>
-          </cell>
-          <cell r="B11">
-            <v>72674.41</v>
-          </cell>
-          <cell r="C11">
-            <v>161290.32999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>LRANGE_100 (first 100 elements)</v>
-          </cell>
-          <cell r="B12">
-            <v>15262.52</v>
-          </cell>
-          <cell r="C12">
-            <v>49019.61</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>LRANGE_300 (first 300 elements)</v>
-          </cell>
-          <cell r="B13">
-            <v>5015.8</v>
-          </cell>
-          <cell r="C13">
-            <v>21008.400000000001</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>LRANGE_500 (first 450 elements)</v>
-          </cell>
-          <cell r="B14">
-            <v>3430.06</v>
-          </cell>
-          <cell r="C14">
-            <v>14684.29</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>LRANGE_600 (first 600 elements)</v>
-          </cell>
-          <cell r="B15">
-            <v>2614.7199999999998</v>
-          </cell>
-          <cell r="C15">
-            <v>11312.22</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>MSET (10 keys)</v>
-          </cell>
-          <cell r="B16">
-            <v>12923.24</v>
-          </cell>
-          <cell r="C16">
-            <v>54347.82</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="redis" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ardb" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ardb" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="redis_1" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="redis" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1200,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1211,133 +1194,161 @@
     <col min="1" max="1" width="28.375" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>90682.38</v>
+        <v>95075.11</v>
       </c>
       <c r="C2">
-        <v>90020.34</v>
+        <v>91945.56</v>
       </c>
       <c r="D2">
-        <v>76523.39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>92274.76</v>
+      </c>
+      <c r="E2">
+        <v>79669.850000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>92039.51</v>
+        <v>99265.43</v>
       </c>
       <c r="C3">
-        <v>92506.94</v>
+        <v>92988.66</v>
       </c>
       <c r="D3">
-        <v>87438.58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>95721.27</v>
+      </c>
+      <c r="E3">
+        <v>90044.66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>49030.18</v>
+        <v>62361.64</v>
       </c>
       <c r="C4">
-        <v>62066.71</v>
+        <v>72490.03</v>
       </c>
       <c r="D4">
-        <v>71850.44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>55567.91</v>
+      </c>
+      <c r="E4">
+        <v>73692.509999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>50949.18</v>
+        <v>69045.990000000005</v>
       </c>
       <c r="C5">
-        <v>87973.19</v>
+        <v>93805.119999999995</v>
       </c>
       <c r="D5">
-        <v>79349.960000000006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>68078.16</v>
+      </c>
+      <c r="E5">
+        <v>82459.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>32067.83</v>
+        <v>47572.160000000003</v>
       </c>
       <c r="C6">
-        <v>48217.17</v>
+        <v>59805.03</v>
       </c>
       <c r="D6">
-        <v>79298.37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>34883.32</v>
+      </c>
+      <c r="E6">
+        <v>74940.61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>26702.13</v>
+        <v>47369.57</v>
       </c>
       <c r="C7">
-        <v>15689.55</v>
+        <v>27713.11</v>
       </c>
       <c r="D7">
-        <v>77643.97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>40584.42</v>
+      </c>
+      <c r="E7">
+        <v>105466.32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>7395.19</v>
+        <v>14205.29</v>
       </c>
       <c r="C8">
-        <v>9658.43</v>
+        <v>14711.51</v>
       </c>
       <c r="D8">
-        <v>77026.77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>10088.27</v>
+      </c>
+      <c r="E8">
+        <v>105797.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>11958.49</v>
+        <v>37583.39</v>
       </c>
       <c r="C9">
-        <v>16065.06</v>
+        <v>41779.82</v>
       </c>
       <c r="D9">
-        <v>76780.740000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>24421.81</v>
+      </c>
+      <c r="E9">
+        <v>100405.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1345,93 +1356,114 @@
         <v>109.32599999999999</v>
       </c>
       <c r="C10">
-        <v>17067.09</v>
+        <v>17614.32</v>
       </c>
       <c r="D10">
-        <v>70997.52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>87.634</v>
+      </c>
+      <c r="E10">
+        <v>75253.039999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>19161.13</v>
+        <v>49504.95</v>
       </c>
       <c r="C11">
-        <v>15705.01</v>
+        <v>16998.71</v>
       </c>
       <c r="D11">
-        <v>79808.460000000006</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>40719.93</v>
+      </c>
+      <c r="E11">
+        <v>87989.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12">
-        <v>6796.99</v>
+        <v>7981.99</v>
       </c>
       <c r="C12">
-        <v>13343.12</v>
+        <v>17639.79</v>
       </c>
       <c r="D12">
-        <v>38269.61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>7445.68</v>
+      </c>
+      <c r="E12">
+        <v>45831.61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
-        <v>2374.41</v>
+        <v>3829.91</v>
       </c>
       <c r="C13">
-        <v>4751.47</v>
+        <v>6578.86</v>
       </c>
       <c r="D13">
-        <v>15735.71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>3113.99</v>
+      </c>
+      <c r="E13">
+        <v>17608.11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14">
-        <v>1650.37</v>
+        <v>2504.61</v>
       </c>
       <c r="C14">
-        <v>3004.68</v>
+        <v>4552.0600000000004</v>
       </c>
       <c r="D14">
-        <v>12432.77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>2156.08</v>
+      </c>
+      <c r="E14">
+        <v>12345.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15">
-        <v>1345.24</v>
+        <v>1734.72</v>
       </c>
       <c r="C15">
-        <v>2505.98</v>
+        <v>3082.94</v>
       </c>
       <c r="D15">
-        <v>9586.19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>1650.46</v>
+      </c>
+      <c r="E15">
+        <v>7906.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16">
-        <v>5472.67</v>
+        <v>9675.48</v>
       </c>
       <c r="C16">
-        <v>4794.2299999999996</v>
+        <v>7204.56</v>
       </c>
       <c r="D16">
+        <v>5255.44</v>
+      </c>
+      <c r="E16">
         <v>35967.599999999999</v>
       </c>
     </row>

</xml_diff>